<commit_message>
test: test case for register event Fixes #233
</commit_message>
<xml_diff>
--- a/__fixtures__/simple-multisheet.xlsx
+++ b/__fixtures__/simple-multisheet.xlsx
@@ -441,17 +441,23 @@
       <c r="A2" t="str">
         <v>Sample Community</v>
       </c>
+      <c r="B2" t="str">
+        <v>{"membershipFee":null,"membershipEmail":null}</v>
+      </c>
       <c r="C2" t="str">
         <v>[{"name":"Membership Carry Forward","hidden":false},{"name":"Summer Festival","hidden":false},{"name":"Corn Roast","hidden":false}]</v>
       </c>
       <c r="D2" t="str">
-        <v>[{"name":"meal","count":null,"unitPrice":null,"hidden":false},{"name":"drink","count":null,"unitPrice":null,"hidden":false},{"name":"cotton-candy","count":null,"unitPrice":null,"hidden":false}]</v>
+        <v>[{"name":"meal","count":null,"unitPrice":"5.00","hidden":false},{"name":"drink","count":null,"unitPrice":"1.00","hidden":false},{"name":"cotton-candy","count":null,"unitPrice":null,"hidden":false}]</v>
       </c>
       <c r="E2" t="str">
         <v>[{"name":"cash","hidden":false},{"name":"e-Transfer","hidden":false},{"name":"free","hidden":false}]</v>
       </c>
       <c r="H2" t="str">
-        <v>2025-09-26T17:46:03.846Z</v>
+        <v>2025-09-29T18:29:07.690Z</v>
+      </c>
+      <c r="I2" t="str">
+        <v>dev@email.com</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: reorder tab after add/remove contact (#234)
</commit_message>
<xml_diff>
--- a/__fixtures__/simple-multisheet.xlsx
+++ b/__fixtures__/simple-multisheet.xlsx
@@ -441,17 +441,23 @@
       <c r="A2" t="str">
         <v>Sample Community</v>
       </c>
+      <c r="B2" t="str">
+        <v>{"membershipFee":null,"membershipEmail":null}</v>
+      </c>
       <c r="C2" t="str">
         <v>[{"name":"Membership Carry Forward","hidden":false},{"name":"Summer Festival","hidden":false},{"name":"Corn Roast","hidden":false}]</v>
       </c>
       <c r="D2" t="str">
-        <v>[{"name":"meal","count":null,"unitPrice":null,"hidden":false},{"name":"drink","count":null,"unitPrice":null,"hidden":false},{"name":"cotton-candy","count":null,"unitPrice":null,"hidden":false}]</v>
+        <v>[{"name":"meal","count":null,"unitPrice":"5.00","hidden":false},{"name":"drink","count":null,"unitPrice":"1.00","hidden":false},{"name":"cotton-candy","count":null,"unitPrice":null,"hidden":false}]</v>
       </c>
       <c r="E2" t="str">
         <v>[{"name":"cash","hidden":false},{"name":"e-Transfer","hidden":false},{"name":"free","hidden":false}]</v>
       </c>
       <c r="H2" t="str">
-        <v>2025-09-26T17:46:03.846Z</v>
+        <v>2025-09-29T18:29:07.690Z</v>
+      </c>
+      <c r="I2" t="str">
+        <v>dev@email.com</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: change database schema for occupancyInfoList
</commit_message>
<xml_diff>
--- a/__fixtures__/simple-multisheet.xlsx
+++ b/__fixtures__/simple-multisheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kendrick/Documents/git/community-db/__fixtures__/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F4E531-7E5F-674C-8F89-14E5877ABA79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F9D662-6126-6B4F-B41E-E242B28E7CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="600" windowWidth="49580" windowHeight="28200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1660" yWindow="600" windowWidth="49540" windowHeight="28200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Community" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="99">
   <si>
     <t>name</t>
   </si>
@@ -320,18 +320,6 @@
   </si>
   <si>
     <t>5</t>
-  </si>
-  <si>
-    <t>Previous</t>
-  </si>
-  <si>
-    <t>Owner</t>
-  </si>
-  <si>
-    <t>2021-12-10T00:00:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-01-23T00:00:00.000Z</t>
   </si>
   <si>
     <t>Sample Community</t>
@@ -713,7 +701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -750,7 +738,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -884,10 +872,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -925,9 +913,6 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>-1</v>
-      </c>
       <c r="D2" t="s">
         <v>41</v>
       </c>
@@ -950,9 +935,6 @@
       </c>
       <c r="B3">
         <v>2</v>
-      </c>
-      <c r="C3">
-        <v>-1</v>
       </c>
       <c r="D3" t="s">
         <v>44</v>
@@ -977,9 +959,6 @@
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4">
-        <v>-1</v>
-      </c>
       <c r="D4" t="s">
         <v>46</v>
       </c>
@@ -1003,9 +982,6 @@
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5">
-        <v>-1</v>
-      </c>
       <c r="D5" t="s">
         <v>48</v>
       </c>
@@ -1017,38 +993,12 @@
       </c>
       <c r="H5" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
-        <v>98</v>
-      </c>
-      <c r="E6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
-        <v>100</v>
-      </c>
-      <c r="H6" t="s">
-        <v>101</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:H5" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:H1 A5:B5 A2:B2 D2:H2 A3:B3 D3:H3 A4:B4 D4:H4 D5:H5" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>